<commit_message>
risk1:research:real-learning:Record configuration vs learning outcomes in csv
Allows you to tweak the network and see the results
</commit_message>
<xml_diff>
--- a/ListenLearn.xlsx
+++ b/ListenLearn.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Spectrum Learning" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>Scenario</t>
   </si>
@@ -32,6 +33,21 @@
   </si>
   <si>
     <t>Relative Epochs</t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>Momentum</t>
+  </si>
+  <si>
+    <t>l1</t>
+  </si>
+  <si>
+    <t>Attempt</t>
+  </si>
+  <si>
+    <t>Epoc</t>
   </si>
 </sst>
 </file>
@@ -375,7 +391,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -508,4 +524,107 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>0.1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>2964</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>0.1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1248</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>0.1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>3055</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>